<commit_message>
Updated layout and BOM with new balun
</commit_message>
<xml_diff>
--- a/JDB-001/BOM/Bill of Materials-JDB-001.xlsx
+++ b/JDB-001/BOM/Bill of Materials-JDB-001.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="296" uniqueCount="257">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="296" uniqueCount="256">
   <si>
     <t xml:space="preserve"> </t>
   </si>
@@ -133,10 +133,10 @@
     <t>None</t>
   </si>
   <si>
-    <t>6/7/2016</t>
-  </si>
-  <si>
-    <t>3:44:00 PM</t>
+    <t>6/13/2016</t>
+  </si>
+  <si>
+    <t>9:07:52 AM</t>
   </si>
   <si>
     <t>Description</t>
@@ -265,7 +265,7 @@
     <t>IC SOC 2.4GHZ 256K FLASH 48QFN</t>
   </si>
   <si>
-    <t>IC BALUN FOR NRF51822 WLCSP</t>
+    <t>NORDIC NRF51 BALUN FILTER</t>
   </si>
   <si>
     <t>IC ERM/LRA HAPTIC DRIVER 9DSBGA</t>
@@ -346,9 +346,6 @@
     <t>Nordic Semiconductor ASA</t>
   </si>
   <si>
-    <t>STMicroelectronics</t>
-  </si>
-  <si>
     <t>Texas Instruments</t>
   </si>
   <si>
@@ -409,7 +406,7 @@
     <t>CDBU0520</t>
   </si>
   <si>
-    <t>SESD0402P1BN-0450-090CT-ND, SESD0402P1BN-0450-090, SESD0402P1BN-0450-090</t>
+    <t>SESD0402P1BN-0450-090</t>
   </si>
   <si>
     <t>BM02B-SURS-TF(LF)(SN)</t>
@@ -481,7 +478,7 @@
     <t>NRF51822-QFAC-R</t>
   </si>
   <si>
-    <t>BAL-NRF02D3</t>
+    <t>2450BM14E0003T</t>
   </si>
   <si>
     <t>DRV2604LYZFR</t>
@@ -763,7 +760,7 @@
     <t>2.33310</t>
   </si>
   <si>
-    <t>0.32000</t>
+    <t>0.66000</t>
   </si>
   <si>
     <t>1.35000</t>
@@ -809,7 +806,6 @@
     <font>
       <sz val="10"/>
       <name val="Arial"/>
-      <family val="2"/>
     </font>
     <font>
       <b/>
@@ -1320,6 +1316,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1333,7 +1330,6 @@
     <xf numFmtId="0" fontId="8" fillId="3" borderId="18" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
@@ -1687,12 +1683,12 @@
       <c r="J1" s="6"/>
     </row>
     <row r="2" spans="1:10" ht="37.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A2" s="77" t="s">
+      <c r="A2" s="78" t="s">
         <v>18</v>
       </c>
-      <c r="B2" s="78"/>
-      <c r="C2" s="79" t="s">
-        <v>254</v>
+      <c r="B2" s="79"/>
+      <c r="C2" s="80" t="s">
+        <v>253</v>
       </c>
       <c r="D2" s="56">
         <v>1</v>
@@ -1739,8 +1735,8 @@
       </c>
       <c r="C5" s="32"/>
       <c r="D5" s="5"/>
-      <c r="E5" s="80" t="s">
-        <v>255</v>
+      <c r="E5" s="75" t="s">
+        <v>254</v>
       </c>
       <c r="F5" s="7"/>
       <c r="G5" s="2"/>
@@ -1790,11 +1786,11 @@
       <c r="A9" s="42"/>
       <c r="B9" s="10">
         <f ca="1">TODAY()</f>
-        <v>42528</v>
+        <v>42534</v>
       </c>
       <c r="C9" s="11">
         <f ca="1">NOW()</f>
-        <v>42528.656954166669</v>
+        <v>42534.382658564813</v>
       </c>
       <c r="D9" s="9"/>
       <c r="E9" s="9"/>
@@ -1832,16 +1828,16 @@
         <v>88</v>
       </c>
       <c r="D12" s="57" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E12" s="61" t="s">
+        <v>159</v>
+      </c>
+      <c r="F12" s="62" t="s">
         <v>160</v>
       </c>
-      <c r="F12" s="62" t="s">
-        <v>161</v>
-      </c>
-      <c r="G12" s="75" t="s">
-        <v>210</v>
+      <c r="G12" s="76" t="s">
+        <v>209</v>
       </c>
       <c r="H12" s="72" t="s">
         <v>34</v>
@@ -1858,16 +1854,16 @@
         <v>89</v>
       </c>
       <c r="D13" s="58" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="E13" s="51">
         <v>1</v>
       </c>
       <c r="F13" s="60" t="s">
-        <v>162</v>
-      </c>
-      <c r="G13" s="76" t="s">
-        <v>211</v>
+        <v>161</v>
+      </c>
+      <c r="G13" s="77" t="s">
+        <v>210</v>
       </c>
       <c r="H13" s="71">
         <f t="shared" ref="H13:H60" si="0">E13*G13</f>
@@ -1885,16 +1881,16 @@
         <v>90</v>
       </c>
       <c r="D14" s="58" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="E14" s="51">
         <v>8</v>
       </c>
       <c r="F14" s="60" t="s">
-        <v>163</v>
-      </c>
-      <c r="G14" s="76" t="s">
-        <v>212</v>
+        <v>162</v>
+      </c>
+      <c r="G14" s="77" t="s">
+        <v>211</v>
       </c>
       <c r="H14" s="71">
         <f t="shared" si="0"/>
@@ -1912,16 +1908,16 @@
         <v>91</v>
       </c>
       <c r="D15" s="58" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="E15" s="51">
         <v>2</v>
       </c>
       <c r="F15" s="60" t="s">
-        <v>164</v>
-      </c>
-      <c r="G15" s="76" t="s">
-        <v>213</v>
+        <v>163</v>
+      </c>
+      <c r="G15" s="77" t="s">
+        <v>212</v>
       </c>
       <c r="H15" s="71">
         <f t="shared" si="0"/>
@@ -1939,16 +1935,16 @@
         <v>90</v>
       </c>
       <c r="D16" s="58" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="E16" s="51">
         <v>1</v>
       </c>
       <c r="F16" s="60" t="s">
-        <v>165</v>
-      </c>
-      <c r="G16" s="76" t="s">
-        <v>214</v>
+        <v>164</v>
+      </c>
+      <c r="G16" s="77" t="s">
+        <v>213</v>
       </c>
       <c r="H16" s="71">
         <f t="shared" si="0"/>
@@ -1966,16 +1962,16 @@
         <v>92</v>
       </c>
       <c r="D17" s="58" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="E17" s="51">
         <v>2</v>
       </c>
       <c r="F17" s="60" t="s">
-        <v>166</v>
-      </c>
-      <c r="G17" s="76" t="s">
-        <v>215</v>
+        <v>165</v>
+      </c>
+      <c r="G17" s="77" t="s">
+        <v>214</v>
       </c>
       <c r="H17" s="71">
         <f t="shared" si="0"/>
@@ -1993,16 +1989,16 @@
         <v>93</v>
       </c>
       <c r="D18" s="58" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="E18" s="51">
         <v>1</v>
       </c>
       <c r="F18" s="60" t="s">
-        <v>167</v>
-      </c>
-      <c r="G18" s="76" t="s">
-        <v>216</v>
+        <v>166</v>
+      </c>
+      <c r="G18" s="77" t="s">
+        <v>215</v>
       </c>
       <c r="H18" s="71">
         <f t="shared" si="0"/>
@@ -2020,16 +2016,16 @@
         <v>90</v>
       </c>
       <c r="D19" s="58" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="E19" s="51">
         <v>1</v>
       </c>
       <c r="F19" s="60" t="s">
-        <v>168</v>
-      </c>
-      <c r="G19" s="76" t="s">
-        <v>217</v>
+        <v>167</v>
+      </c>
+      <c r="G19" s="77" t="s">
+        <v>216</v>
       </c>
       <c r="H19" s="71">
         <f t="shared" si="0"/>
@@ -2047,16 +2043,16 @@
         <v>90</v>
       </c>
       <c r="D20" s="58" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="E20" s="51">
         <v>7</v>
       </c>
       <c r="F20" s="60" t="s">
-        <v>169</v>
-      </c>
-      <c r="G20" s="76" t="s">
-        <v>218</v>
+        <v>168</v>
+      </c>
+      <c r="G20" s="77" t="s">
+        <v>217</v>
       </c>
       <c r="H20" s="71">
         <f t="shared" si="0"/>
@@ -2074,16 +2070,16 @@
         <v>94</v>
       </c>
       <c r="D21" s="58" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="E21" s="51">
         <v>2</v>
       </c>
       <c r="F21" s="60" t="s">
-        <v>170</v>
-      </c>
-      <c r="G21" s="76" t="s">
-        <v>219</v>
+        <v>169</v>
+      </c>
+      <c r="G21" s="77" t="s">
+        <v>218</v>
       </c>
       <c r="H21" s="71">
         <f t="shared" si="0"/>
@@ -2101,16 +2097,16 @@
         <v>91</v>
       </c>
       <c r="D22" s="58" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="E22" s="51">
         <v>5</v>
       </c>
       <c r="F22" s="60" t="s">
-        <v>171</v>
-      </c>
-      <c r="G22" s="76" t="s">
-        <v>220</v>
+        <v>170</v>
+      </c>
+      <c r="G22" s="77" t="s">
+        <v>219</v>
       </c>
       <c r="H22" s="71">
         <f t="shared" si="0"/>
@@ -2128,16 +2124,16 @@
         <v>91</v>
       </c>
       <c r="D23" s="58" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="E23" s="51">
         <v>1</v>
       </c>
       <c r="F23" s="60" t="s">
-        <v>172</v>
-      </c>
-      <c r="G23" s="76" t="s">
-        <v>221</v>
+        <v>171</v>
+      </c>
+      <c r="G23" s="77" t="s">
+        <v>220</v>
       </c>
       <c r="H23" s="71">
         <f t="shared" si="0"/>
@@ -2155,16 +2151,16 @@
         <v>90</v>
       </c>
       <c r="D24" s="58" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="E24" s="51">
         <v>1</v>
       </c>
       <c r="F24" s="60" t="s">
-        <v>173</v>
-      </c>
-      <c r="G24" s="76" t="s">
-        <v>222</v>
+        <v>172</v>
+      </c>
+      <c r="G24" s="77" t="s">
+        <v>221</v>
       </c>
       <c r="H24" s="71">
         <f t="shared" si="0"/>
@@ -2182,16 +2178,16 @@
         <v>90</v>
       </c>
       <c r="D25" s="58" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="E25" s="51">
         <v>1</v>
       </c>
       <c r="F25" s="60" t="s">
-        <v>174</v>
-      </c>
-      <c r="G25" s="76" t="s">
-        <v>223</v>
+        <v>173</v>
+      </c>
+      <c r="G25" s="77" t="s">
+        <v>222</v>
       </c>
       <c r="H25" s="71">
         <f t="shared" si="0"/>
@@ -2209,16 +2205,16 @@
         <v>95</v>
       </c>
       <c r="D26" s="58" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="E26" s="51">
         <v>4</v>
       </c>
       <c r="F26" s="60" t="s">
-        <v>175</v>
-      </c>
-      <c r="G26" s="76" t="s">
-        <v>224</v>
+        <v>174</v>
+      </c>
+      <c r="G26" s="77" t="s">
+        <v>223</v>
       </c>
       <c r="H26" s="71">
         <f t="shared" si="0"/>
@@ -2236,16 +2232,16 @@
         <v>96</v>
       </c>
       <c r="D27" s="58" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="E27" s="51">
         <v>1</v>
       </c>
       <c r="F27" s="60" t="s">
-        <v>176</v>
-      </c>
-      <c r="G27" s="76" t="s">
-        <v>225</v>
+        <v>175</v>
+      </c>
+      <c r="G27" s="77" t="s">
+        <v>224</v>
       </c>
       <c r="H27" s="71">
         <f t="shared" si="0"/>
@@ -2263,16 +2259,16 @@
         <v>97</v>
       </c>
       <c r="D28" s="58" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="E28" s="51">
         <v>1</v>
       </c>
       <c r="F28" s="60" t="s">
-        <v>177</v>
-      </c>
-      <c r="G28" s="76" t="s">
-        <v>226</v>
+        <v>176</v>
+      </c>
+      <c r="G28" s="77" t="s">
+        <v>225</v>
       </c>
       <c r="H28" s="71">
         <f t="shared" si="0"/>
@@ -2290,16 +2286,16 @@
         <v>98</v>
       </c>
       <c r="D29" s="58" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="E29" s="51">
         <v>3</v>
       </c>
       <c r="F29" s="60" t="s">
-        <v>178</v>
-      </c>
-      <c r="G29" s="76" t="s">
-        <v>227</v>
+        <v>177</v>
+      </c>
+      <c r="G29" s="77" t="s">
+        <v>226</v>
       </c>
       <c r="H29" s="71">
         <f t="shared" si="0"/>
@@ -2317,16 +2313,16 @@
         <v>99</v>
       </c>
       <c r="D30" s="58" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="E30" s="51">
         <v>2</v>
       </c>
       <c r="F30" s="60" t="s">
-        <v>179</v>
-      </c>
-      <c r="G30" s="76" t="s">
-        <v>228</v>
+        <v>178</v>
+      </c>
+      <c r="G30" s="77" t="s">
+        <v>227</v>
       </c>
       <c r="H30" s="71">
         <f t="shared" si="0"/>
@@ -2344,16 +2340,16 @@
         <v>100</v>
       </c>
       <c r="D31" s="58" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="E31" s="51">
         <v>1</v>
       </c>
       <c r="F31" s="60" t="s">
-        <v>180</v>
-      </c>
-      <c r="G31" s="76" t="s">
-        <v>229</v>
+        <v>179</v>
+      </c>
+      <c r="G31" s="77" t="s">
+        <v>228</v>
       </c>
       <c r="H31" s="71">
         <f t="shared" si="0"/>
@@ -2371,16 +2367,16 @@
         <v>91</v>
       </c>
       <c r="D32" s="58" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="E32" s="51">
         <v>1</v>
       </c>
       <c r="F32" s="60" t="s">
-        <v>181</v>
-      </c>
-      <c r="G32" s="76" t="s">
-        <v>230</v>
+        <v>180</v>
+      </c>
+      <c r="G32" s="77" t="s">
+        <v>229</v>
       </c>
       <c r="H32" s="71">
         <f t="shared" si="0"/>
@@ -2398,16 +2394,16 @@
         <v>94</v>
       </c>
       <c r="D33" s="58" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="E33" s="51">
         <v>1</v>
       </c>
       <c r="F33" s="60" t="s">
-        <v>182</v>
-      </c>
-      <c r="G33" s="76" t="s">
-        <v>231</v>
+        <v>181</v>
+      </c>
+      <c r="G33" s="77" t="s">
+        <v>230</v>
       </c>
       <c r="H33" s="71">
         <f t="shared" si="0"/>
@@ -2425,16 +2421,16 @@
         <v>101</v>
       </c>
       <c r="D34" s="58" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="E34" s="51">
         <v>4</v>
       </c>
       <c r="F34" s="60" t="s">
-        <v>183</v>
-      </c>
-      <c r="G34" s="76" t="s">
-        <v>232</v>
+        <v>182</v>
+      </c>
+      <c r="G34" s="77" t="s">
+        <v>231</v>
       </c>
       <c r="H34" s="71">
         <f t="shared" si="0"/>
@@ -2452,16 +2448,16 @@
         <v>102</v>
       </c>
       <c r="D35" s="58" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="E35" s="51">
         <v>1</v>
       </c>
       <c r="F35" s="60" t="s">
-        <v>184</v>
-      </c>
-      <c r="G35" s="76" t="s">
-        <v>233</v>
+        <v>183</v>
+      </c>
+      <c r="G35" s="77" t="s">
+        <v>232</v>
       </c>
       <c r="H35" s="71">
         <f t="shared" si="0"/>
@@ -2479,16 +2475,16 @@
         <v>103</v>
       </c>
       <c r="D36" s="58" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="E36" s="51">
         <v>1</v>
       </c>
       <c r="F36" s="60" t="s">
-        <v>185</v>
-      </c>
-      <c r="G36" s="76" t="s">
-        <v>234</v>
+        <v>184</v>
+      </c>
+      <c r="G36" s="77" t="s">
+        <v>233</v>
       </c>
       <c r="H36" s="71">
         <f t="shared" si="0"/>
@@ -2506,16 +2502,16 @@
         <v>104</v>
       </c>
       <c r="D37" s="58" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="E37" s="51">
         <v>1</v>
       </c>
       <c r="F37" s="60" t="s">
-        <v>186</v>
-      </c>
-      <c r="G37" s="76" t="s">
-        <v>235</v>
+        <v>185</v>
+      </c>
+      <c r="G37" s="77" t="s">
+        <v>234</v>
       </c>
       <c r="H37" s="71">
         <f t="shared" si="0"/>
@@ -2533,16 +2529,16 @@
         <v>91</v>
       </c>
       <c r="D38" s="58" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="E38" s="51">
         <v>1</v>
       </c>
       <c r="F38" s="60" t="s">
-        <v>187</v>
-      </c>
-      <c r="G38" s="76" t="s">
-        <v>236</v>
+        <v>186</v>
+      </c>
+      <c r="G38" s="77" t="s">
+        <v>235</v>
       </c>
       <c r="H38" s="71">
         <f t="shared" si="0"/>
@@ -2560,16 +2556,16 @@
         <v>91</v>
       </c>
       <c r="D39" s="58" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="E39" s="51">
         <v>2</v>
       </c>
       <c r="F39" s="60" t="s">
-        <v>188</v>
-      </c>
-      <c r="G39" s="76" t="s">
-        <v>237</v>
+        <v>187</v>
+      </c>
+      <c r="G39" s="77" t="s">
+        <v>236</v>
       </c>
       <c r="H39" s="71">
         <f t="shared" si="0"/>
@@ -2587,16 +2583,16 @@
         <v>103</v>
       </c>
       <c r="D40" s="58" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="E40" s="51">
         <v>5</v>
       </c>
       <c r="F40" s="60" t="s">
-        <v>189</v>
-      </c>
-      <c r="G40" s="76" t="s">
-        <v>238</v>
+        <v>188</v>
+      </c>
+      <c r="G40" s="77" t="s">
+        <v>237</v>
       </c>
       <c r="H40" s="71">
         <f t="shared" si="0"/>
@@ -2614,16 +2610,16 @@
         <v>105</v>
       </c>
       <c r="D41" s="58" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="E41" s="51">
         <v>1</v>
       </c>
       <c r="F41" s="60" t="s">
-        <v>190</v>
-      </c>
-      <c r="G41" s="76" t="s">
-        <v>239</v>
+        <v>189</v>
+      </c>
+      <c r="G41" s="77" t="s">
+        <v>238</v>
       </c>
       <c r="H41" s="71">
         <f t="shared" si="0"/>
@@ -2641,16 +2637,16 @@
         <v>105</v>
       </c>
       <c r="D42" s="58" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="E42" s="51">
         <v>1</v>
       </c>
       <c r="F42" s="60" t="s">
-        <v>191</v>
-      </c>
-      <c r="G42" s="76" t="s">
-        <v>239</v>
+        <v>190</v>
+      </c>
+      <c r="G42" s="77" t="s">
+        <v>238</v>
       </c>
       <c r="H42" s="71">
         <f t="shared" si="0"/>
@@ -2668,16 +2664,16 @@
         <v>105</v>
       </c>
       <c r="D43" s="58" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="E43" s="51">
         <v>1</v>
       </c>
       <c r="F43" s="60" t="s">
-        <v>192</v>
-      </c>
-      <c r="G43" s="76" t="s">
-        <v>239</v>
+        <v>191</v>
+      </c>
+      <c r="G43" s="77" t="s">
+        <v>238</v>
       </c>
       <c r="H43" s="71">
         <f t="shared" si="0"/>
@@ -2695,16 +2691,16 @@
         <v>103</v>
       </c>
       <c r="D44" s="58" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="E44" s="51">
         <v>1</v>
       </c>
       <c r="F44" s="60" t="s">
-        <v>193</v>
-      </c>
-      <c r="G44" s="76" t="s">
-        <v>240</v>
+        <v>192</v>
+      </c>
+      <c r="G44" s="77" t="s">
+        <v>239</v>
       </c>
       <c r="H44" s="71">
         <f t="shared" si="0"/>
@@ -2722,16 +2718,16 @@
         <v>103</v>
       </c>
       <c r="D45" s="58" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="E45" s="51">
         <v>1</v>
       </c>
       <c r="F45" s="60" t="s">
-        <v>194</v>
-      </c>
-      <c r="G45" s="76" t="s">
-        <v>241</v>
+        <v>193</v>
+      </c>
+      <c r="G45" s="77" t="s">
+        <v>240</v>
       </c>
       <c r="H45" s="71">
         <f t="shared" si="0"/>
@@ -2749,16 +2745,16 @@
         <v>105</v>
       </c>
       <c r="D46" s="58" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="E46" s="51">
         <v>1</v>
       </c>
       <c r="F46" s="60" t="s">
-        <v>195</v>
-      </c>
-      <c r="G46" s="76" t="s">
-        <v>239</v>
+        <v>194</v>
+      </c>
+      <c r="G46" s="77" t="s">
+        <v>238</v>
       </c>
       <c r="H46" s="71">
         <f t="shared" si="0"/>
@@ -2776,16 +2772,16 @@
         <v>105</v>
       </c>
       <c r="D47" s="58" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="E47" s="51">
         <v>1</v>
       </c>
       <c r="F47" s="60" t="s">
-        <v>196</v>
-      </c>
-      <c r="G47" s="76" t="s">
-        <v>236</v>
+        <v>195</v>
+      </c>
+      <c r="G47" s="77" t="s">
+        <v>235</v>
       </c>
       <c r="H47" s="71">
         <f t="shared" si="0"/>
@@ -2803,16 +2799,16 @@
         <v>91</v>
       </c>
       <c r="D48" s="58" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="E48" s="51">
         <v>1</v>
       </c>
       <c r="F48" s="60" t="s">
-        <v>197</v>
-      </c>
-      <c r="G48" s="76" t="s">
-        <v>242</v>
+        <v>196</v>
+      </c>
+      <c r="G48" s="77" t="s">
+        <v>241</v>
       </c>
       <c r="H48" s="71">
         <f t="shared" si="0"/>
@@ -2830,16 +2826,16 @@
         <v>103</v>
       </c>
       <c r="D49" s="58" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="E49" s="51">
         <v>2</v>
       </c>
       <c r="F49" s="60" t="s">
-        <v>198</v>
-      </c>
-      <c r="G49" s="76" t="s">
-        <v>243</v>
+        <v>197</v>
+      </c>
+      <c r="G49" s="77" t="s">
+        <v>242</v>
       </c>
       <c r="H49" s="71">
         <f t="shared" si="0"/>
@@ -2857,16 +2853,16 @@
         <v>92</v>
       </c>
       <c r="D50" s="58" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="E50" s="51">
         <v>2</v>
       </c>
       <c r="F50" s="60" t="s">
-        <v>199</v>
-      </c>
-      <c r="G50" s="76" t="s">
-        <v>215</v>
+        <v>198</v>
+      </c>
+      <c r="G50" s="77" t="s">
+        <v>214</v>
       </c>
       <c r="H50" s="71">
         <f t="shared" si="0"/>
@@ -2884,16 +2880,16 @@
         <v>90</v>
       </c>
       <c r="D51" s="58" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="E51" s="51">
         <v>1</v>
       </c>
       <c r="F51" s="60" t="s">
-        <v>200</v>
-      </c>
-      <c r="G51" s="76" t="s">
-        <v>244</v>
+        <v>199</v>
+      </c>
+      <c r="G51" s="77" t="s">
+        <v>243</v>
       </c>
       <c r="H51" s="71">
         <f t="shared" si="0"/>
@@ -2911,16 +2907,16 @@
         <v>106</v>
       </c>
       <c r="D52" s="58" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="E52" s="51">
         <v>2</v>
       </c>
       <c r="F52" s="60" t="s">
-        <v>201</v>
-      </c>
-      <c r="G52" s="76" t="s">
-        <v>245</v>
+        <v>200</v>
+      </c>
+      <c r="G52" s="77" t="s">
+        <v>244</v>
       </c>
       <c r="H52" s="71">
         <f t="shared" si="0"/>
@@ -2938,16 +2934,16 @@
         <v>107</v>
       </c>
       <c r="D53" s="58" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="E53" s="51">
         <v>1</v>
       </c>
       <c r="F53" s="60" t="s">
-        <v>202</v>
-      </c>
-      <c r="G53" s="76" t="s">
-        <v>246</v>
+        <v>201</v>
+      </c>
+      <c r="G53" s="77" t="s">
+        <v>245</v>
       </c>
       <c r="H53" s="71">
         <f t="shared" si="0"/>
@@ -2962,23 +2958,23 @@
         <v>81</v>
       </c>
       <c r="C54" s="58" t="s">
-        <v>108</v>
+        <v>89</v>
       </c>
       <c r="D54" s="58" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="E54" s="51">
         <v>1</v>
       </c>
       <c r="F54" s="60" t="s">
-        <v>203</v>
-      </c>
-      <c r="G54" s="76" t="s">
-        <v>247</v>
+        <v>202</v>
+      </c>
+      <c r="G54" s="77" t="s">
+        <v>246</v>
       </c>
       <c r="H54" s="71">
         <f t="shared" si="0"/>
-        <v>0.32</v>
+        <v>0.66</v>
       </c>
     </row>
     <row r="55" spans="1:10" s="12" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.4">
@@ -2989,19 +2985,19 @@
         <v>82</v>
       </c>
       <c r="C55" s="58" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D55" s="58" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="E55" s="51">
         <v>1</v>
       </c>
       <c r="F55" s="60" t="s">
-        <v>204</v>
-      </c>
-      <c r="G55" s="76" t="s">
-        <v>248</v>
+        <v>203</v>
+      </c>
+      <c r="G55" s="77" t="s">
+        <v>247</v>
       </c>
       <c r="H55" s="71">
         <f t="shared" si="0"/>
@@ -3016,19 +3012,19 @@
         <v>83</v>
       </c>
       <c r="C56" s="58" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D56" s="58" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="E56" s="51">
         <v>1</v>
       </c>
       <c r="F56" s="60" t="s">
-        <v>205</v>
-      </c>
-      <c r="G56" s="76" t="s">
-        <v>249</v>
+        <v>204</v>
+      </c>
+      <c r="G56" s="77" t="s">
+        <v>248</v>
       </c>
       <c r="H56" s="71">
         <f t="shared" si="0"/>
@@ -3043,19 +3039,19 @@
         <v>84</v>
       </c>
       <c r="C57" s="58" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D57" s="58" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="E57" s="51">
         <v>1</v>
       </c>
       <c r="F57" s="60" t="s">
-        <v>206</v>
-      </c>
-      <c r="G57" s="76" t="s">
-        <v>250</v>
+        <v>205</v>
+      </c>
+      <c r="G57" s="77" t="s">
+        <v>249</v>
       </c>
       <c r="H57" s="71">
         <f t="shared" si="0"/>
@@ -3070,19 +3066,19 @@
         <v>85</v>
       </c>
       <c r="C58" s="58" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D58" s="58" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="E58" s="51">
         <v>1</v>
       </c>
       <c r="F58" s="60" t="s">
-        <v>207</v>
-      </c>
-      <c r="G58" s="76" t="s">
-        <v>251</v>
+        <v>206</v>
+      </c>
+      <c r="G58" s="77" t="s">
+        <v>250</v>
       </c>
       <c r="H58" s="71">
         <f t="shared" si="0"/>
@@ -3097,19 +3093,19 @@
         <v>86</v>
       </c>
       <c r="C59" s="58" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D59" s="58" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="E59" s="51">
         <v>1</v>
       </c>
       <c r="F59" s="60" t="s">
-        <v>208</v>
-      </c>
-      <c r="G59" s="76" t="s">
-        <v>252</v>
+        <v>207</v>
+      </c>
+      <c r="G59" s="77" t="s">
+        <v>251</v>
       </c>
       <c r="H59" s="71">
         <f t="shared" si="0"/>
@@ -3124,19 +3120,19 @@
         <v>87</v>
       </c>
       <c r="C60" s="58" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D60" s="58" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="E60" s="51">
         <v>1</v>
       </c>
       <c r="F60" s="60" t="s">
-        <v>209</v>
-      </c>
-      <c r="G60" s="76" t="s">
-        <v>253</v>
+        <v>208</v>
+      </c>
+      <c r="G60" s="77" t="s">
+        <v>252</v>
       </c>
       <c r="H60" s="71">
         <f t="shared" si="0"/>
@@ -3151,10 +3147,10 @@
       <c r="F61" s="44"/>
       <c r="H61" s="81">
         <f>SUM(H13:H60)</f>
-        <v>26.896880000000003</v>
+        <v>27.236879999999999</v>
       </c>
       <c r="I61" s="82" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="J61" s="6"/>
     </row>

</xml_diff>